<commit_message>
finish panel plotting and PCA for proximate nutrient
</commit_message>
<xml_diff>
--- a/carb/input_carb/carb_weights.xlsx
+++ b/carb/input_carb/carb_weights.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trevo\OneDrive\Documents\GitHub\TEdissy_analysis\carb\input_carb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C5188E-0DC3-4362-9A5E-D092011223BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8077AD-8E18-46CB-88BE-D72FC2B8184E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{DAA52A09-508C-4E60-B9E1-D2DB41C7A14E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>Lab_65</t>
+  </si>
+  <si>
+    <t>absorbance</t>
   </si>
 </sst>
 </file>
@@ -477,15 +480,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04654F25-0708-40A6-A168-13F9737EF41A}">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -501,8 +504,11 @@
       <c r="E1">
         <v>750</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -518,8 +524,12 @@
       <c r="E2">
         <v>1.0999999999999999E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2">
+        <f>D2-E2</f>
+        <v>0.61799999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -535,8 +545,12 @@
       <c r="E3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3">
+        <f t="shared" ref="F3:F47" si="0">D3-E3</f>
+        <v>0.64800000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -552,8 +566,12 @@
       <c r="E4">
         <v>4.2000000000000003E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -569,8 +587,12 @@
       <c r="E5">
         <v>1.7999999999999999E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0.60399999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -586,8 +608,12 @@
       <c r="E6">
         <v>6.5000000000000002E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0.59800000000000009</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -603,8 +629,12 @@
       <c r="E7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0.56299999999999994</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -620,8 +650,12 @@
       <c r="E8">
         <v>7.1999999999999995E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0.58100000000000007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -637,8 +671,12 @@
       <c r="E9">
         <v>8.0000000000000002E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0.54400000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -654,8 +692,12 @@
       <c r="E10">
         <v>2.8000000000000001E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0.47699999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -671,8 +713,12 @@
       <c r="E11">
         <v>5.5E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0.61699999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -688,8 +734,12 @@
       <c r="E12">
         <v>6.5000000000000002E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0.67700000000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -705,8 +755,12 @@
       <c r="E13">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0.62399999999999989</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -722,8 +776,12 @@
       <c r="E14">
         <v>6.9000000000000006E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0.53499999999999992</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -739,8 +797,12 @@
       <c r="E15">
         <v>4.8000000000000001E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>0.56899999999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -756,8 +818,12 @@
       <c r="E16">
         <v>7.8E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>0.63100000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -773,8 +839,12 @@
       <c r="E17">
         <v>2.8999999999999998E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>0.82409999999999994</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -790,8 +860,12 @@
       <c r="E18">
         <v>6.2E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>0.66900000000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -807,8 +881,12 @@
       <c r="E19">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>0.41700000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -824,8 +902,12 @@
       <c r="E20">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>0.65900000000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -841,8 +923,12 @@
       <c r="E21">
         <v>0.16300000000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>0.65299999999999991</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -858,8 +944,12 @@
       <c r="E22">
         <v>1.7999999999999999E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>0.65200000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -875,8 +965,12 @@
       <c r="E23">
         <v>6.6000000000000003E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>0.64300000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -892,8 +986,12 @@
       <c r="E24">
         <v>7.4999999999999997E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>0.63700000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -909,8 +1007,12 @@
       <c r="E25">
         <v>6.3E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>0.65300000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -926,8 +1028,12 @@
       <c r="E26">
         <v>0.223</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>0.623</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -943,8 +1049,12 @@
       <c r="E27">
         <v>9.7000000000000003E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>0.82500000000000007</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -960,8 +1070,12 @@
       <c r="E28">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>0.85499999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -977,8 +1091,12 @@
       <c r="E29">
         <v>0.27600000000000002</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>0.82000000000000006</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -994,8 +1112,12 @@
       <c r="E30">
         <v>0.189</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>0.74199999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -1011,8 +1133,12 @@
       <c r="E31">
         <v>8.3000000000000004E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>0.94399999999999995</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -1028,8 +1154,12 @@
       <c r="E32">
         <v>6.2E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>1.115</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -1045,8 +1175,12 @@
       <c r="E33">
         <v>0.105</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>0.83100000000000007</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -1062,8 +1196,12 @@
       <c r="E34">
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>0.504</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -1079,8 +1217,12 @@
       <c r="E35">
         <v>7.4999999999999997E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -1096,8 +1238,12 @@
       <c r="E36">
         <v>4.1000000000000002E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>0.67999999999999994</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -1113,8 +1259,12 @@
       <c r="E37">
         <v>2.9000000000000001E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>0.68899999999999995</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -1130,8 +1280,12 @@
       <c r="E38">
         <v>6.0999999999999999E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>0.64399999999999991</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>16</v>
       </c>
@@ -1147,8 +1301,12 @@
       <c r="E39">
         <v>0.156</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>0.47699999999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -1164,8 +1322,12 @@
       <c r="E40">
         <v>4.3999999999999997E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>0.45800000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>10</v>
       </c>
@@ -1181,8 +1343,12 @@
       <c r="E41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>0.46600000000000003</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -1198,8 +1364,12 @@
       <c r="E42">
         <v>2.5999999999999999E-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>0.51600000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>17</v>
       </c>
@@ -1215,8 +1385,12 @@
       <c r="E43">
         <v>2.1999999999999999E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>17</v>
       </c>
@@ -1232,8 +1406,12 @@
       <c r="E44">
         <v>3.9E-2</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F44">
+        <f t="shared" si="0"/>
+        <v>0.56399999999999995</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -1249,8 +1427,12 @@
       <c r="E45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>0.496</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>18</v>
       </c>
@@ -1266,8 +1448,12 @@
       <c r="E46">
         <v>0.111</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F46">
+        <f t="shared" si="0"/>
+        <v>0.82699999999999996</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>18</v>
       </c>
@@ -1282,6 +1468,10 @@
       </c>
       <c r="E47">
         <v>0.111</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="0"/>
+        <v>0.746</v>
       </c>
     </row>
   </sheetData>

</xml_diff>